<commit_message>
added analysis for netbeans
</commit_message>
<xml_diff>
--- a/eclipse/analysis/analysis_2002_2004.xlsx
+++ b/eclipse/analysis/analysis_2002_2004.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P146"/>
+  <dimension ref="A1:Q146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,6 +434,11 @@
           <t>OI Layer 3</t>
         </is>
       </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>OI Layer 4</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -494,6 +499,9 @@
       <c r="P2" t="n">
         <v>4.125181544872829</v>
       </c>
+      <c r="Q2" t="n">
+        <v>5.791233729379734</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -554,6 +562,9 @@
       <c r="P3" t="n">
         <v>4.191311846145393</v>
       </c>
+      <c r="Q3" t="n">
+        <v>5.75288078808115</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -614,6 +625,9 @@
       <c r="P4" t="n">
         <v>3.823490543706778</v>
       </c>
+      <c r="Q4" t="n">
+        <v>5.767549891852452</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -674,6 +688,9 @@
       <c r="P5" t="n">
         <v>3.885759837759023</v>
       </c>
+      <c r="Q5" t="n">
+        <v>5.787818938051471</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -734,6 +751,9 @@
       <c r="P6" t="n">
         <v>3.38116911287208</v>
       </c>
+      <c r="Q6" t="n">
+        <v>5.509426758983825</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -794,6 +814,9 @@
       <c r="P7" t="n">
         <v>3.733957364735724</v>
       </c>
+      <c r="Q7" t="n">
+        <v>5.770897696735526</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -854,6 +877,9 @@
       <c r="P8" t="n">
         <v>3.854984545218969</v>
       </c>
+      <c r="Q8" t="n">
+        <v>5.787359974080999</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -914,6 +940,9 @@
       <c r="P9" t="n">
         <v>4.007505075063323</v>
       </c>
+      <c r="Q9" t="n">
+        <v>5.78715346378314</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -974,6 +1003,9 @@
       <c r="P10" t="n">
         <v>3.1436191440596</v>
       </c>
+      <c r="Q10" t="n">
+        <v>5.770897696735526</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1034,6 +1066,9 @@
       <c r="P11" t="n">
         <v>3.432737787210531</v>
       </c>
+      <c r="Q11" t="n">
+        <v>5.5012858527397</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1094,6 +1129,9 @@
       <c r="P12" t="n">
         <v>3.733507743248415</v>
       </c>
+      <c r="Q12" t="n">
+        <v>5.788688299736727</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1154,6 +1192,9 @@
       <c r="P13" t="n">
         <v>4.05736351766103</v>
       </c>
+      <c r="Q13" t="n">
+        <v>5.785838065782305</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1214,6 +1255,9 @@
       <c r="P14" t="n">
         <v>4.175869214525506</v>
       </c>
+      <c r="Q14" t="n">
+        <v>5.786612390845653</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1274,6 +1318,9 @@
       <c r="P15" t="n">
         <v>3.845796384891004</v>
       </c>
+      <c r="Q15" t="n">
+        <v>5.765965054655419</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1334,6 +1381,9 @@
       <c r="P16" t="n">
         <v>3.833243685424841</v>
       </c>
+      <c r="Q16" t="n">
+        <v>5.786977722164827</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1394,6 +1444,9 @@
       <c r="P17" t="n">
         <v>4.106030254105453</v>
       </c>
+      <c r="Q17" t="n">
+        <v>5.767843658627354</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1454,6 +1507,9 @@
       <c r="P18" t="n">
         <v>3.999768057337133</v>
       </c>
+      <c r="Q18" t="n">
+        <v>5.791160348082275</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1514,6 +1570,9 @@
       <c r="P19" t="n">
         <v>3.959808781501476</v>
       </c>
+      <c r="Q19" t="n">
+        <v>5.790524522121557</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1574,6 +1633,9 @@
       <c r="P20" t="n">
         <v>4.071270649724665</v>
       </c>
+      <c r="Q20" t="n">
+        <v>5.787812858655856</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1634,6 +1696,9 @@
       <c r="P21" t="n">
         <v>3.445409679484099</v>
       </c>
+      <c r="Q21" t="n">
+        <v>5.765319248886385</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1694,6 +1759,9 @@
       <c r="P22" t="n">
         <v>4.03238140944632</v>
       </c>
+      <c r="Q22" t="n">
+        <v>5.770897696735526</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1754,6 +1822,9 @@
       <c r="P23" t="n">
         <v>4.151782551460408</v>
       </c>
+      <c r="Q23" t="n">
+        <v>5.789122118674877</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1814,6 +1885,9 @@
       <c r="P24" t="n">
         <v>4.135204080735088</v>
       </c>
+      <c r="Q24" t="n">
+        <v>5.768972507644656</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1874,6 +1948,9 @@
       <c r="P25" t="n">
         <v>3.991978460117508</v>
       </c>
+      <c r="Q25" t="n">
+        <v>5.769180227004989</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1934,6 +2011,9 @@
       <c r="P26" t="n">
         <v>4.108007784126979</v>
       </c>
+      <c r="Q26" t="n">
+        <v>5.790384737974954</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1994,6 +2074,9 @@
       <c r="P27" t="n">
         <v>3.835390415890187</v>
       </c>
+      <c r="Q27" t="n">
+        <v>5.771414670186291</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2054,6 +2137,9 @@
       <c r="P28" t="n">
         <v>2.969411656558471</v>
       </c>
+      <c r="Q28" t="n">
+        <v>5.584897292895866</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2114,6 +2200,9 @@
       <c r="P29" t="n">
         <v>3.796003372563474</v>
       </c>
+      <c r="Q29" t="n">
+        <v>5.766602998983003</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -2174,6 +2263,9 @@
       <c r="P30" t="n">
         <v>3.255194417790982</v>
       </c>
+      <c r="Q30" t="n">
+        <v>5.790223844338691</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -2234,6 +2326,9 @@
       <c r="P31" t="n">
         <v>3.977337705426009</v>
       </c>
+      <c r="Q31" t="n">
+        <v>5.787204512486868</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -2294,6 +2389,9 @@
       <c r="P32" t="n">
         <v>3.824305112570109</v>
       </c>
+      <c r="Q32" t="n">
+        <v>5.783981195772091</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2354,6 +2452,9 @@
       <c r="P33" t="n">
         <v>3.783897964326782</v>
       </c>
+      <c r="Q33" t="n">
+        <v>5.785481865093068</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2414,6 +2515,9 @@
       <c r="P34" t="n">
         <v>3.565431262273071</v>
       </c>
+      <c r="Q34" t="n">
+        <v>5.789137694748367</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -2474,6 +2578,9 @@
       <c r="P35" t="n">
         <v>3.408618564898188</v>
       </c>
+      <c r="Q35" t="n">
+        <v>5.536347698038263</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -2534,6 +2641,9 @@
       <c r="P36" t="n">
         <v>3.912203844102562</v>
       </c>
+      <c r="Q36" t="n">
+        <v>5.768069795775451</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2594,6 +2704,9 @@
       <c r="P37" t="n">
         <v>3.84397120360673</v>
       </c>
+      <c r="Q37" t="n">
+        <v>5.790223844338691</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -2654,6 +2767,9 @@
       <c r="P38" t="n">
         <v>4.164103788112536</v>
       </c>
+      <c r="Q38" t="n">
+        <v>5.770546852815471</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -2714,6 +2830,9 @@
       <c r="P39" t="n">
         <v>3.769729788262828</v>
       </c>
+      <c r="Q39" t="n">
+        <v>5.790794662737971</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -2774,6 +2893,9 @@
       <c r="P40" t="n">
         <v>4.032316525366974</v>
       </c>
+      <c r="Q40" t="n">
+        <v>5.78798358055282</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -2834,6 +2956,9 @@
       <c r="P41" t="n">
         <v>3.406965743032771</v>
       </c>
+      <c r="Q41" t="n">
+        <v>5.691306163593389</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -2894,6 +3019,9 @@
       <c r="P42" t="n">
         <v>3.98383305460404</v>
       </c>
+      <c r="Q42" t="n">
+        <v>5.779565751165346</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -2954,6 +3082,9 @@
       <c r="P43" t="n">
         <v>3.461660188852829</v>
       </c>
+      <c r="Q43" t="n">
+        <v>5.765588990846803</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -3014,6 +3145,9 @@
       <c r="P44" t="n">
         <v>3.358266908027171</v>
       </c>
+      <c r="Q44" t="n">
+        <v>5.789122118674876</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -3074,6 +3208,9 @@
       <c r="P45" t="n">
         <v>4.018330358174666</v>
       </c>
+      <c r="Q45" t="n">
+        <v>5.784149131741579</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -3134,6 +3271,9 @@
       <c r="P46" t="n">
         <v>4.014568540699765</v>
       </c>
+      <c r="Q46" t="n">
+        <v>5.785140829268625</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -3194,6 +3334,9 @@
       <c r="P47" t="n">
         <v>3.93817312521798</v>
       </c>
+      <c r="Q47" t="n">
+        <v>5.789137694748367</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -3254,6 +3397,9 @@
       <c r="P48" t="n">
         <v>3.526278808386211</v>
       </c>
+      <c r="Q48" t="n">
+        <v>5.765319248886386</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -3314,6 +3460,9 @@
       <c r="P49" t="n">
         <v>1.953626637613183</v>
       </c>
+      <c r="Q49" t="n">
+        <v>5.715246642412993</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -3374,6 +3523,9 @@
       <c r="P50" t="n">
         <v>2.200733312265555</v>
       </c>
+      <c r="Q50" t="n">
+        <v>5.715246642412992</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -3434,6 +3586,9 @@
       <c r="P51" t="n">
         <v>2.744686970574509</v>
       </c>
+      <c r="Q51" t="n">
+        <v>5.791447785482061</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -3494,6 +3649,9 @@
       <c r="P52" t="n">
         <v>3.470075242808264</v>
       </c>
+      <c r="Q52" t="n">
+        <v>5.140851173568478</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -3554,6 +3712,9 @@
       <c r="P53" t="n">
         <v>3.8677932746735</v>
       </c>
+      <c r="Q53" t="n">
+        <v>5.788059272800817</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -3614,6 +3775,9 @@
       <c r="P54" t="n">
         <v>3.556649012487183</v>
       </c>
+      <c r="Q54" t="n">
+        <v>5.790546477632047</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -3674,6 +3838,9 @@
       <c r="P55" t="n">
         <v>3.224453434102601</v>
       </c>
+      <c r="Q55" t="n">
+        <v>5.783299859563927</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -3734,6 +3901,9 @@
       <c r="P56" t="n">
         <v>3.785180061028556</v>
       </c>
+      <c r="Q56" t="n">
+        <v>5.790582341529334</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -3794,6 +3964,9 @@
       <c r="P57" t="n">
         <v>1.302571169075077</v>
       </c>
+      <c r="Q57" t="n">
+        <v>5.137130269738939</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -3854,6 +4027,9 @@
       <c r="P58" t="n">
         <v>3.954539846485788</v>
       </c>
+      <c r="Q58" t="n">
+        <v>5.783299859563927</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -3914,6 +4090,9 @@
       <c r="P59" t="n">
         <v>3.713585229268923</v>
       </c>
+      <c r="Q59" t="n">
+        <v>5.716220679239032</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -3974,6 +4153,9 @@
       <c r="P60" t="n">
         <v>3.985963704470659</v>
       </c>
+      <c r="Q60" t="n">
+        <v>5.78820329439954</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -4034,6 +4216,9 @@
       <c r="P61" t="n">
         <v>1.926740944002768</v>
       </c>
+      <c r="Q61" t="n">
+        <v>5.765895386107436</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -4094,6 +4279,9 @@
       <c r="P62" t="n">
         <v>3.7202178342173</v>
       </c>
+      <c r="Q62" t="n">
+        <v>5.780272107937174</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -4154,6 +4342,9 @@
       <c r="P63" t="n">
         <v>3.903889728772266</v>
       </c>
+      <c r="Q63" t="n">
+        <v>5.780455782696637</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -4214,6 +4405,9 @@
       <c r="P64" t="n">
         <v>4.069059432936743</v>
       </c>
+      <c r="Q64" t="n">
+        <v>5.784976958593262</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -4274,6 +4468,9 @@
       <c r="P65" t="n">
         <v>3.862734275418432</v>
       </c>
+      <c r="Q65" t="n">
+        <v>5.787204512486866</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -4334,6 +4531,9 @@
       <c r="P66" t="n">
         <v>4.12373765531604</v>
       </c>
+      <c r="Q66" t="n">
+        <v>5.790007454527229</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -4394,6 +4594,9 @@
       <c r="P67" t="n">
         <v>3.681767537155411</v>
       </c>
+      <c r="Q67" t="n">
+        <v>5.764864307201424</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -4454,6 +4657,9 @@
       <c r="P68" t="n">
         <v>4.168801066249451</v>
       </c>
+      <c r="Q68" t="n">
+        <v>5.77679074696196</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -4514,6 +4720,9 @@
       <c r="P69" t="n">
         <v>4.007977296682691</v>
       </c>
+      <c r="Q69" t="n">
+        <v>5.78597746424616</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -4574,6 +4783,9 @@
       <c r="P70" t="n">
         <v>4.094262216685864</v>
       </c>
+      <c r="Q70" t="n">
+        <v>5.784976958593264</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -4634,6 +4846,9 @@
       <c r="P71" t="n">
         <v>4.063836165139939</v>
       </c>
+      <c r="Q71" t="n">
+        <v>5.781028793581628</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -4694,6 +4909,9 @@
       <c r="P72" t="n">
         <v>3.764647854910424</v>
       </c>
+      <c r="Q72" t="n">
+        <v>5.786967474086267</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -4754,6 +4972,9 @@
       <c r="P73" t="n">
         <v>3.752555855761595</v>
       </c>
+      <c r="Q73" t="n">
+        <v>5.78548186509307</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -4814,6 +5035,9 @@
       <c r="P74" t="n">
         <v>4.036740263193555</v>
       </c>
+      <c r="Q74" t="n">
+        <v>5.789912031610754</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -4874,6 +5098,9 @@
       <c r="P75" t="n">
         <v>1.610055511644576</v>
       </c>
+      <c r="Q75" t="n">
+        <v>5.614876445462961</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -4934,6 +5161,9 @@
       <c r="P76" t="n">
         <v>4.02851086192249</v>
       </c>
+      <c r="Q76" t="n">
+        <v>5.788786066249338</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -4994,6 +5224,9 @@
       <c r="P77" t="n">
         <v>3.696182527915698</v>
       </c>
+      <c r="Q77" t="n">
+        <v>5.788786066249338</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -5054,6 +5287,9 @@
       <c r="P78" t="n">
         <v>3.714951466901957</v>
       </c>
+      <c r="Q78" t="n">
+        <v>5.789122118674876</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -5114,6 +5350,9 @@
       <c r="P79" t="n">
         <v>2.820584383345881</v>
       </c>
+      <c r="Q79" t="n">
+        <v>5.790794662737971</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -5174,6 +5413,9 @@
       <c r="P80" t="n">
         <v>3.488021169256909</v>
       </c>
+      <c r="Q80" t="n">
+        <v>5.765895386107434</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -5234,6 +5476,9 @@
       <c r="P81" t="n">
         <v>3.737556486460721</v>
       </c>
+      <c r="Q81" t="n">
+        <v>5.765895386107436</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -5294,6 +5539,9 @@
       <c r="P82" t="n">
         <v>3.821348366667666</v>
       </c>
+      <c r="Q82" t="n">
+        <v>5.790384737974955</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -5354,6 +5602,9 @@
       <c r="P83" t="n">
         <v>3.183336946683211</v>
       </c>
+      <c r="Q83" t="n">
+        <v>5.788786066249336</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -5414,6 +5665,9 @@
       <c r="P84" t="n">
         <v>3.147601549991981</v>
       </c>
+      <c r="Q84" t="n">
+        <v>5.783299859563927</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -5474,6 +5728,9 @@
       <c r="P85" t="n">
         <v>3.817388662896989</v>
       </c>
+      <c r="Q85" t="n">
+        <v>5.790915112016457</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -5534,6 +5791,9 @@
       <c r="P86" t="n">
         <v>4.005767071321023</v>
       </c>
+      <c r="Q86" t="n">
+        <v>5.783299859563928</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -5594,6 +5854,9 @@
       <c r="P87" t="n">
         <v>3.844729076164661</v>
       </c>
+      <c r="Q87" t="n">
+        <v>5.791447785482061</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -5654,6 +5917,9 @@
       <c r="P88" t="n">
         <v>3.944369224818368</v>
       </c>
+      <c r="Q88" t="n">
+        <v>5.79022384433869</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -5714,6 +5980,9 @@
       <c r="P89" t="n">
         <v>4.063386605513895</v>
       </c>
+      <c r="Q89" t="n">
+        <v>5.77679074696196</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -5774,6 +6043,9 @@
       <c r="P90" t="n">
         <v>3.843459591103768</v>
       </c>
+      <c r="Q90" t="n">
+        <v>5.789912031610754</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -5834,6 +6106,9 @@
       <c r="P91" t="n">
         <v>3.695006430149665</v>
       </c>
+      <c r="Q91" t="n">
+        <v>5.765895386107436</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -5894,6 +6169,9 @@
       <c r="P92" t="n">
         <v>4.134391405015954</v>
       </c>
+      <c r="Q92" t="n">
+        <v>5.780457807500697</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -5954,6 +6232,9 @@
       <c r="P93" t="n">
         <v>3.931139156229466</v>
       </c>
+      <c r="Q93" t="n">
+        <v>5.788296405717084</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -6014,6 +6295,9 @@
       <c r="P94" t="n">
         <v>3.338928865048314</v>
       </c>
+      <c r="Q94" t="n">
+        <v>5.78323999993876</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -6074,6 +6358,9 @@
       <c r="P95" t="n">
         <v>3.525834359621886</v>
       </c>
+      <c r="Q95" t="n">
+        <v>5.765743403497133</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -6134,6 +6421,9 @@
       <c r="P96" t="n">
         <v>3.83052127750836</v>
       </c>
+      <c r="Q96" t="n">
+        <v>5.770659677347785</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -6194,6 +6484,9 @@
       <c r="P97" t="n">
         <v>3.363634891338492</v>
       </c>
+      <c r="Q97" t="n">
+        <v>5.443392994975627</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -6254,6 +6547,9 @@
       <c r="P98" t="n">
         <v>3.854231099832474</v>
       </c>
+      <c r="Q98" t="n">
+        <v>5.771144377050531</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -6314,6 +6610,9 @@
       <c r="P99" t="n">
         <v>3.84067040426408</v>
       </c>
+      <c r="Q99" t="n">
+        <v>5.784976958593264</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -6374,6 +6673,9 @@
       <c r="P100" t="n">
         <v>3.16836023571185</v>
       </c>
+      <c r="Q100" t="n">
+        <v>5.720874641084169</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -6434,6 +6736,9 @@
       <c r="P101" t="n">
         <v>2.44563777635972</v>
       </c>
+      <c r="Q101" t="n">
+        <v>5.503548083882775</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -6494,6 +6799,9 @@
       <c r="P102" t="n">
         <v>3.281736668133984</v>
       </c>
+      <c r="Q102" t="n">
+        <v>5.791447785482061</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -6554,6 +6862,9 @@
       <c r="P103" t="n">
         <v>3.718504990261684</v>
       </c>
+      <c r="Q103" t="n">
+        <v>5.790794662737971</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -6614,6 +6925,9 @@
       <c r="P104" t="n">
         <v>3.97317041908076</v>
       </c>
+      <c r="Q104" t="n">
+        <v>5.790223844338692</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -6674,6 +6988,9 @@
       <c r="P105" t="n">
         <v>2.633692967427636</v>
       </c>
+      <c r="Q105" t="n">
+        <v>5.765895386107436</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -6734,6 +7051,9 @@
       <c r="P106" t="n">
         <v>3.115011028935792</v>
       </c>
+      <c r="Q106" t="n">
+        <v>5.781345971769182</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -6794,6 +7114,9 @@
       <c r="P107" t="n">
         <v>3.312956347789141</v>
       </c>
+      <c r="Q107" t="n">
+        <v>5.783299859563927</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -6854,6 +7177,9 @@
       <c r="P108" t="n">
         <v>2.305142728366103</v>
       </c>
+      <c r="Q108" t="n">
+        <v>5.765895386107436</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -6914,6 +7240,9 @@
       <c r="P109" t="n">
         <v>2.846899081167756</v>
       </c>
+      <c r="Q109" t="n">
+        <v>5.655233219641977</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -6974,6 +7303,9 @@
       <c r="P110" t="n">
         <v>3.731817464127386</v>
       </c>
+      <c r="Q110" t="n">
+        <v>5.781712314819092</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -7034,6 +7366,9 @@
       <c r="P111" t="n">
         <v>2.511785288242135</v>
       </c>
+      <c r="Q111" t="n">
+        <v>5.739587493613701</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -7094,6 +7429,9 @@
       <c r="P112" t="n">
         <v>2.243131695650112</v>
       </c>
+      <c r="Q112" t="n">
+        <v>5.790794662737971</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -7154,6 +7492,9 @@
       <c r="P113" t="n">
         <v>3.950458388319105</v>
       </c>
+      <c r="Q113" t="n">
+        <v>5.790794662737971</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -7214,6 +7555,9 @@
       <c r="P114" t="n">
         <v>4.028410474975908</v>
       </c>
+      <c r="Q114" t="n">
+        <v>5.786612390845653</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -7274,6 +7618,9 @@
       <c r="P115" t="n">
         <v>3.873514060075923</v>
       </c>
+      <c r="Q115" t="n">
+        <v>5.787818938051471</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -7334,6 +7681,9 @@
       <c r="P116" t="n">
         <v>2.836803238539071</v>
       </c>
+      <c r="Q116" t="n">
+        <v>5.719221676819869</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -7394,6 +7744,9 @@
       <c r="P117" t="n">
         <v>3.183211738067946</v>
       </c>
+      <c r="Q117" t="n">
+        <v>5.765895386107426</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -7454,6 +7807,9 @@
       <c r="P118" t="n">
         <v>2.17139039099435</v>
       </c>
+      <c r="Q118" t="n">
+        <v>5.790794662737971</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -7514,6 +7870,9 @@
       <c r="P119" t="n">
         <v>3.651369757766607</v>
       </c>
+      <c r="Q119" t="n">
+        <v>5.791447785482061</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -7574,6 +7933,9 @@
       <c r="P120" t="n">
         <v>3.942459484460225</v>
       </c>
+      <c r="Q120" t="n">
+        <v>5.790794662737971</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -7634,6 +7996,9 @@
       <c r="P121" t="n">
         <v>3.361645687844069</v>
       </c>
+      <c r="Q121" t="n">
+        <v>5.739419306505999</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -7694,6 +8059,9 @@
       <c r="P122" t="n">
         <v>4.042462673017592</v>
       </c>
+      <c r="Q122" t="n">
+        <v>5.790223844338691</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -7754,6 +8122,9 @@
       <c r="P123" t="n">
         <v>3.281623969631646</v>
       </c>
+      <c r="Q123" t="n">
+        <v>5.651703638623507</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -7814,6 +8185,9 @@
       <c r="P124" t="n">
         <v>1.995032354373053</v>
       </c>
+      <c r="Q124" t="n">
+        <v>5.715246642412993</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -7874,6 +8248,9 @@
       <c r="P125" t="n">
         <v>3.661324327761154</v>
       </c>
+      <c r="Q125" t="n">
+        <v>5.790384737974956</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -7934,6 +8311,9 @@
       <c r="P126" t="n">
         <v>3.917479332116216</v>
       </c>
+      <c r="Q126" t="n">
+        <v>5.781712314819091</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -7994,6 +8374,9 @@
       <c r="P127" t="n">
         <v>3.214283431674793</v>
       </c>
+      <c r="Q127" t="n">
+        <v>5.783299859563928</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -8054,6 +8437,9 @@
       <c r="P128" t="n">
         <v>4.084881287420544</v>
       </c>
+      <c r="Q128" t="n">
+        <v>5.789122118674876</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -8114,6 +8500,9 @@
       <c r="P129" t="n">
         <v>3.460128366397486</v>
       </c>
+      <c r="Q129" t="n">
+        <v>5.767044878116788</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -8174,6 +8563,9 @@
       <c r="P130" t="n">
         <v>2.826813720666912</v>
       </c>
+      <c r="Q130" t="n">
+        <v>5.770897696735525</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -8234,6 +8626,9 @@
       <c r="P131" t="n">
         <v>3.696438276786989</v>
       </c>
+      <c r="Q131" t="n">
+        <v>5.788059272800816</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -8294,6 +8689,9 @@
       <c r="P132" t="n">
         <v>3.925613320735256</v>
       </c>
+      <c r="Q132" t="n">
+        <v>5.789076123356136</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
@@ -8354,6 +8752,9 @@
       <c r="P133" t="n">
         <v>3.730188443667957</v>
       </c>
+      <c r="Q133" t="n">
+        <v>5.790812401285461</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -8414,6 +8815,9 @@
       <c r="P134" t="n">
         <v>3.224050808681782</v>
       </c>
+      <c r="Q134" t="n">
+        <v>5.770452130604641</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -8474,6 +8878,9 @@
       <c r="P135" t="n">
         <v>4.064091741890851</v>
       </c>
+      <c r="Q135" t="n">
+        <v>5.789272326876127</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -8534,6 +8941,9 @@
       <c r="P136" t="n">
         <v>3.725337531736547</v>
       </c>
+      <c r="Q136" t="n">
+        <v>5.790915112016457</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -8594,6 +9004,9 @@
       <c r="P137" t="n">
         <v>4.224921925455178</v>
       </c>
+      <c r="Q137" t="n">
+        <v>5.789122118674876</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -8654,6 +9067,9 @@
       <c r="P138" t="n">
         <v>3.721194632218162</v>
       </c>
+      <c r="Q138" t="n">
+        <v>5.770897696735521</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -8714,6 +9130,9 @@
       <c r="P139" t="n">
         <v>3.296043338504877</v>
       </c>
+      <c r="Q139" t="n">
+        <v>5.79022384433869</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -8774,6 +9193,9 @@
       <c r="P140" t="n">
         <v>4.16645284958314</v>
       </c>
+      <c r="Q140" t="n">
+        <v>5.78507054862808</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -8834,6 +9256,9 @@
       <c r="P141" t="n">
         <v>4.133714098591817</v>
       </c>
+      <c r="Q141" t="n">
+        <v>5.789122118674876</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -8894,6 +9319,9 @@
       <c r="P142" t="n">
         <v>4.076273564419742</v>
       </c>
+      <c r="Q142" t="n">
+        <v>5.789122118674876</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -8954,6 +9382,9 @@
       <c r="P143" t="n">
         <v>3.942297991926865</v>
       </c>
+      <c r="Q143" t="n">
+        <v>5.770897696735526</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -9014,6 +9445,9 @@
       <c r="P144" t="n">
         <v>3.991069402269803</v>
       </c>
+      <c r="Q144" t="n">
+        <v>5.790915112016457</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -9074,6 +9508,9 @@
       <c r="P145" t="n">
         <v>3.921080420130924</v>
       </c>
+      <c r="Q145" t="n">
+        <v>5.781741688830164</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -9133,6 +9570,9 @@
       </c>
       <c r="P146" t="n">
         <v>3.580424206201296</v>
+      </c>
+      <c r="Q146" t="n">
+        <v>5.722711962372325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>